<commit_message>
Se agregó archivo .env, se generan logs de aplicacion y se mejoró la tolerancia a fallos
</commit_message>
<xml_diff>
--- a/reportes.xlsx
+++ b/reportes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\OneDrive\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fernando\OneDrive\Escritorio\automatizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3F9109-762E-42E7-9E7E-49D24BB5B8F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF94526D-A75C-4895-8D8E-63587792C404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="4020" windowWidth="20460" windowHeight="10770" xr2:uid="{D2CC3BBF-7243-4963-8FD0-C792BCC390CA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Usuario</t>
   </si>
@@ -62,10 +62,13 @@
     <t>atenasfrar@hotmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">Campaña </t>
-  </si>
-  <si>
     <t>fernandonarea27@hotmail.com</t>
+  </si>
+  <si>
+    <t>fernandonarea6@gmail.com</t>
+  </si>
+  <si>
+    <t>Campaña</t>
   </si>
 </sst>
 </file>
@@ -122,10 +125,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -165,11 +170,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF90F6D9-A24E-42A8-843D-80EB0EB83837}" name="Tabla1" displayName="Tabla1" ref="A1:D3" totalsRowShown="0">
-  <autoFilter ref="A1:D3" xr:uid="{CF90F6D9-A24E-42A8-843D-80EB0EB83837}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF90F6D9-A24E-42A8-843D-80EB0EB83837}" name="Tabla1" displayName="Tabla1" ref="A1:D4" totalsRowShown="0">
+  <autoFilter ref="A1:D4" xr:uid="{CF90F6D9-A24E-42A8-843D-80EB0EB83837}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{1F74779A-28E9-4B9B-B39F-7B81CA43336A}" name="Usuario" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="2" xr3:uid="{E74D0827-7E70-4FA3-8A8C-358DC72A1649}" name="Campaña " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{E74D0827-7E70-4FA3-8A8C-358DC72A1649}" name="Campaña" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{4510F1FF-6E4A-430C-A880-6165E6599449}" name="Incidencias"/>
     <tableColumn id="4" xr3:uid="{4E5E6561-A832-459A-B527-C5411E5B3B62}" name="Nombre Archivo"/>
   </tableColumns>
@@ -497,7 +502,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +518,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -524,7 +529,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -551,23 +556,37 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>654</v>
+      </c>
+      <c r="D4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
+      <c r="D6" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{A8989C89-FE75-439D-9EA2-B8E38F17CEA4}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{C60D1985-E63A-4679-9302-91C6542E3966}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{9618F64E-CB45-4020-A988-BD819E9E449F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>